<commit_message>
Calendario y clases - Ver Perfil del usuario
</commit_message>
<xml_diff>
--- a/src/main/webapp/factura/ingresos.xlsx
+++ b/src/main/webapp/factura/ingresos.xlsx
@@ -177,7 +177,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n" s="2">
-        <v>600.0</v>
+        <v>819.0</v>
       </c>
     </row>
     <row r="6">
@@ -188,7 +188,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="n" s="2">
-        <v>3176.0</v>
+        <v>3245.0</v>
       </c>
     </row>
     <row r="7">
@@ -199,7 +199,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="n" s="2">
-        <v>300.0</v>
+        <v>369.0</v>
       </c>
     </row>
     <row r="8">
@@ -219,7 +219,7 @@
       </c>
       <c r="C11" s="1" t="str">
         <f>SUBTOTAL(109,C2:C8)</f>
-        <v>S/.7376.00</v>
+        <v>S/.7733.00</v>
       </c>
     </row>
   </sheetData>

</xml_diff>